<commit_message>
adding tech choices to dashboard
</commit_message>
<xml_diff>
--- a/app/outputs/partner_match.xlsx
+++ b/app/outputs/partner_match.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="83">
   <si>
     <t>Partners</t>
   </si>
@@ -28,58 +28,238 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>Access Afya</t>
+  </si>
+  <si>
+    <t>American Family Insurance Institute for Corporate and Social Impact</t>
+  </si>
+  <si>
     <t>American Student Assistance (ASA)</t>
   </si>
   <si>
+    <t>Americares</t>
+  </si>
+  <si>
+    <t>Antropia ESSEC</t>
+  </si>
+  <si>
+    <t>AutoCognita</t>
+  </si>
+  <si>
+    <t>Best Buy</t>
+  </si>
+  <si>
+    <t>Blue Haven Initiative</t>
+  </si>
+  <si>
     <t>BMW Foundation Herbert Quandt</t>
   </si>
   <si>
+    <t>Cambridge Associates</t>
+  </si>
+  <si>
+    <t>Capital One</t>
+  </si>
+  <si>
+    <t>Care 2 Communities</t>
+  </si>
+  <si>
+    <t>Cast Collective</t>
+  </si>
+  <si>
     <t>Clint Taylor</t>
   </si>
   <si>
     <t>Clorox</t>
   </si>
   <si>
+    <t>Closed Loop Partners</t>
+  </si>
+  <si>
+    <t>Comcast NBCUniversal</t>
+  </si>
+  <si>
+    <t>Compassion International</t>
+  </si>
+  <si>
     <t>Conduent</t>
   </si>
   <si>
+    <t>Covestro</t>
+  </si>
+  <si>
+    <t>Danaher</t>
+  </si>
+  <si>
     <t>Deshpande Foundation</t>
   </si>
   <si>
+    <t>Dubai Cares</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>EcoAdvisors</t>
+  </si>
+  <si>
+    <t>EILEEN FISHER</t>
+  </si>
+  <si>
+    <t>Enel Foundation and Strategic Studies Center</t>
+  </si>
+  <si>
     <t>Firefly Innovations</t>
   </si>
   <si>
+    <t>Georgia-Pacific Foundation</t>
+  </si>
+  <si>
+    <t>Gina's Collective</t>
+  </si>
+  <si>
+    <t>Global Fund to fight Aids, Tuberculosis and Malaria</t>
+  </si>
+  <si>
     <t>Grupo Salinas</t>
   </si>
   <si>
+    <t>Henkel</t>
+  </si>
+  <si>
     <t>Ingredion</t>
   </si>
   <si>
+    <t>Innospark Ventures</t>
+  </si>
+  <si>
+    <t>Innovation Norway</t>
+  </si>
+  <si>
     <t>Kevin Przybocki</t>
   </si>
   <si>
+    <t>Klaxoon</t>
+  </si>
+  <si>
+    <t>KSF Impact</t>
+  </si>
+  <si>
+    <t>Leap Ventures</t>
+  </si>
+  <si>
+    <t>Lex Mundi Pro Bono Foundation</t>
+  </si>
+  <si>
     <t>Llamasoft</t>
   </si>
   <si>
+    <t>Mannin Research</t>
+  </si>
+  <si>
+    <t>Merck for Mothers</t>
+  </si>
+  <si>
     <t>Merian Ventures</t>
   </si>
   <si>
+    <t>MIT Club of Northern California</t>
+  </si>
+  <si>
     <t>Mondi Group</t>
   </si>
   <si>
+    <t>Morgridge Family Foundation</t>
+  </si>
+  <si>
+    <t>National Rongxiang Xu Foundation</t>
+  </si>
+  <si>
+    <t>Northrop Grumman Corporation</t>
+  </si>
+  <si>
+    <t>Nuvo</t>
+  </si>
+  <si>
+    <t>Olam International</t>
+  </si>
+  <si>
+    <t>Oliver Wyman Group</t>
+  </si>
+  <si>
+    <t>Penn Foster</t>
+  </si>
+  <si>
     <t>Pfizer Inc.</t>
   </si>
   <si>
+    <t>Queen Rania Foundation for Education and Development</t>
+  </si>
+  <si>
+    <t>RISE</t>
+  </si>
+  <si>
+    <t>Save the Children</t>
+  </si>
+  <si>
+    <t>Seed Global Health</t>
+  </si>
+  <si>
     <t>Someone Else's Child Foundation</t>
   </si>
   <si>
+    <t>Soronko Solutions</t>
+  </si>
+  <si>
+    <t>Sresta Natural Bioproducts Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Stand Together</t>
+  </si>
+  <si>
+    <t>Strada Education Network</t>
+  </si>
+  <si>
+    <t>Tecnológico de Monterrey</t>
+  </si>
+  <si>
+    <t>TGR Foundation</t>
+  </si>
+  <si>
     <t>The Hague Business Agency</t>
   </si>
   <si>
     <t>The Kamath Family Foundation</t>
   </si>
   <si>
+    <t>The Nature Conservancy</t>
+  </si>
+  <si>
+    <t>The Pershing Square Foundation</t>
+  </si>
+  <si>
     <t>Twilio.org</t>
+  </si>
+  <si>
+    <t>Uber</t>
+  </si>
+  <si>
+    <t>Ultranauts Inc</t>
+  </si>
+  <si>
+    <t>UN Women</t>
+  </si>
+  <si>
+    <t>Usizo Advisory Solutions</t>
+  </si>
+  <si>
+    <t>Women’s WorldWide Web (W4)</t>
+  </si>
+  <si>
+    <t>Xprize</t>
+  </si>
+  <si>
+    <t>YUM Brands</t>
   </si>
   <si>
     <t>None</t>
@@ -440,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,13 +645,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -479,13 +659,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -493,13 +673,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -507,13 +687,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -521,13 +701,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -535,13 +715,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -549,13 +729,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -563,13 +743,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -577,13 +757,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -591,13 +771,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -605,13 +785,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -619,13 +799,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -633,13 +813,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -647,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -661,13 +841,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -675,13 +855,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -689,13 +869,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -703,13 +883,853 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>